<commit_message>
Add analysis of C1920-E2
</commit_message>
<xml_diff>
--- a/data/C1920.xlsx
+++ b/data/C1920.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="2" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="15540" windowWidth="25520" xWindow="5860" yWindow="1980"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="5860" yWindow="1980" windowWidth="25520" windowHeight="15540" tabRatio="500" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="E1" sheetId="1" state="visible" r:id="rId1"/>
@@ -11,7 +11,7 @@
     <sheet name="E3" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" concurrentCalc="0" fullCalcOnLoad="1" refMode="R1C1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1" refMode="R1C1" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -53,17 +53,17 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
 </styleSheet>
 </file>
 
@@ -336,17 +336,17 @@
   </sheetPr>
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90">
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="0"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="4" min="4" style="2" width="11.33203125"/>
-    <col customWidth="1" max="7" min="7" style="2" width="18.83203125"/>
+    <col width="11.33203125" bestFit="1" customWidth="1" style="2" min="4" max="4"/>
+    <col width="18.83203125" customWidth="1" style="2" min="7" max="7"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1">
+    <row r="1" customFormat="1" s="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>grupo</t>
@@ -466,7 +466,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" s="2">
+    <row r="5">
       <c r="A5" t="inlineStr">
         <is>
           <t>ESO1D</t>
@@ -733,7 +733,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" s="2">
+    <row r="15">
       <c r="A15" t="inlineStr">
         <is>
           <t>ESO4C</t>
@@ -1307,7 +1307,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1317,19 +1317,19 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="0"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="4" min="4" style="2" width="11.33203125"/>
-    <col customWidth="1" max="7" min="7" style="2" width="18.83203125"/>
+    <col width="11.33203125" bestFit="1" customWidth="1" style="2" min="4" max="4"/>
+    <col width="18.83203125" customWidth="1" style="2" min="7" max="7"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1">
+    <row r="1" customFormat="1" s="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>grupo</t>
@@ -1371,7 +1371,7 @@
         </is>
       </c>
     </row>
-    <row r="2" s="2">
+    <row r="2">
       <c r="A2" t="inlineStr">
         <is>
           <t>ESO1A</t>
@@ -1382,8 +1382,20 @@
           <t>ESO</t>
         </is>
       </c>
-    </row>
-    <row r="3" s="2">
+      <c r="C2" t="n">
+        <v>30.8</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1.42</v>
+      </c>
+      <c r="E2" t="n">
+        <v>4.07</v>
+      </c>
+      <c r="H2" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" t="inlineStr">
         <is>
           <t>ESO1B</t>
@@ -1394,8 +1406,20 @@
           <t>ESO</t>
         </is>
       </c>
-    </row>
-    <row r="4" s="2">
+      <c r="C3" t="n">
+        <v>34.6</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="E3" t="n">
+        <v>4.77</v>
+      </c>
+      <c r="H3" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" t="inlineStr">
         <is>
           <t>ESO1C</t>
@@ -1406,8 +1430,20 @@
           <t>ESO</t>
         </is>
       </c>
-    </row>
-    <row r="5" s="2">
+      <c r="C4" t="n">
+        <v>35.7</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="E4" t="n">
+        <v>3.38</v>
+      </c>
+      <c r="H4" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" t="inlineStr">
         <is>
           <t>ESO1D</t>
@@ -1418,8 +1454,20 @@
           <t>ESO</t>
         </is>
       </c>
-    </row>
-    <row r="6" s="2">
+      <c r="C5" t="n">
+        <v>48.1</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1.69</v>
+      </c>
+      <c r="E5" t="n">
+        <v>5.23</v>
+      </c>
+      <c r="H5" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6" t="inlineStr">
         <is>
           <t>ESO2A</t>
@@ -1430,8 +1478,20 @@
           <t>ESO</t>
         </is>
       </c>
-    </row>
-    <row r="7" s="2">
+      <c r="C6" t="n">
+        <v>56</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1.39</v>
+      </c>
+      <c r="E6" t="n">
+        <v>6.52</v>
+      </c>
+      <c r="H6" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7">
       <c r="A7" t="inlineStr">
         <is>
           <t>ESO2B</t>
@@ -1442,8 +1502,20 @@
           <t>ESO</t>
         </is>
       </c>
-    </row>
-    <row r="8" s="2">
+      <c r="C7" t="n">
+        <v>60</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1.66</v>
+      </c>
+      <c r="E7" t="n">
+        <v>4.77</v>
+      </c>
+      <c r="H7" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8">
       <c r="A8" t="inlineStr">
         <is>
           <t>ESO2C</t>
@@ -1454,8 +1526,20 @@
           <t>ESO</t>
         </is>
       </c>
-    </row>
-    <row r="9" s="2">
+      <c r="C8" t="n">
+        <v>16.7</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="E8" t="n">
+        <v>7.36</v>
+      </c>
+      <c r="H8" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9">
       <c r="A9" t="inlineStr">
         <is>
           <t>ESO3A</t>
@@ -1466,8 +1550,20 @@
           <t>ESO</t>
         </is>
       </c>
-    </row>
-    <row r="10" s="2">
+      <c r="C9" t="n">
+        <v>53.8</v>
+      </c>
+      <c r="D9" t="n">
+        <v>2.04</v>
+      </c>
+      <c r="E9" t="n">
+        <v>3.06</v>
+      </c>
+      <c r="H9" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10">
       <c r="A10" t="inlineStr">
         <is>
           <t>ESO3B</t>
@@ -1478,8 +1574,20 @@
           <t>ESO</t>
         </is>
       </c>
-    </row>
-    <row r="11" s="2">
+      <c r="C10" t="n">
+        <v>30.8</v>
+      </c>
+      <c r="D10" t="n">
+        <v>2.36</v>
+      </c>
+      <c r="E10" t="n">
+        <v>4.74</v>
+      </c>
+      <c r="H10" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11">
       <c r="A11" t="inlineStr">
         <is>
           <t>ESO3C</t>
@@ -1490,8 +1598,20 @@
           <t>ESO</t>
         </is>
       </c>
-    </row>
-    <row r="12" s="2">
+      <c r="C11" t="n">
+        <v>39.3</v>
+      </c>
+      <c r="D11" t="n">
+        <v>2.82</v>
+      </c>
+      <c r="E11" t="n">
+        <v>2.75</v>
+      </c>
+      <c r="H11" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12">
       <c r="A12" t="inlineStr">
         <is>
           <t>ESO3D</t>
@@ -1502,8 +1622,20 @@
           <t>ESO</t>
         </is>
       </c>
-    </row>
-    <row r="13" s="2">
+      <c r="C12" t="n">
+        <v>25</v>
+      </c>
+      <c r="D12" t="n">
+        <v>3.65</v>
+      </c>
+      <c r="E12" t="n">
+        <v>4.85</v>
+      </c>
+      <c r="H12" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13">
       <c r="A13" t="inlineStr">
         <is>
           <t>ESO4A</t>
@@ -1514,8 +1646,20 @@
           <t>ESO</t>
         </is>
       </c>
-    </row>
-    <row r="14" s="2">
+      <c r="C13" t="n">
+        <v>45.8</v>
+      </c>
+      <c r="D13" t="n">
+        <v>4.13</v>
+      </c>
+      <c r="E13" t="n">
+        <v>2.55</v>
+      </c>
+      <c r="H13" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14">
       <c r="A14" t="inlineStr">
         <is>
           <t>ESO4B</t>
@@ -1526,8 +1670,20 @@
           <t>ESO</t>
         </is>
       </c>
-    </row>
-    <row r="15" s="2">
+      <c r="C14" t="n">
+        <v>33.3</v>
+      </c>
+      <c r="D14" t="n">
+        <v>3.01</v>
+      </c>
+      <c r="E14" t="n">
+        <v>3.46</v>
+      </c>
+      <c r="H14" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15">
       <c r="A15" t="inlineStr">
         <is>
           <t>ESO4C</t>
@@ -1537,6 +1693,18 @@
         <is>
           <t>ESO</t>
         </is>
+      </c>
+      <c r="C15" t="n">
+        <v>24</v>
+      </c>
+      <c r="D15" t="n">
+        <v>3.69</v>
+      </c>
+      <c r="E15" t="n">
+        <v>6.99</v>
+      </c>
+      <c r="H15" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="16">
@@ -1550,6 +1718,18 @@
           <t>FPB</t>
         </is>
       </c>
+      <c r="C16" t="n">
+        <v>46.7</v>
+      </c>
+      <c r="D16" t="n">
+        <v>5.53</v>
+      </c>
+      <c r="E16" t="n">
+        <v>20.56</v>
+      </c>
+      <c r="H16" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1562,6 +1742,18 @@
           <t>FPB</t>
         </is>
       </c>
+      <c r="C17" t="n">
+        <v>14.3</v>
+      </c>
+      <c r="D17" t="n">
+        <v>8.67</v>
+      </c>
+      <c r="E17" t="n">
+        <v>20.87</v>
+      </c>
+      <c r="H17" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1574,6 +1766,18 @@
           <t>BACH</t>
         </is>
       </c>
+      <c r="C18" t="n">
+        <v>29.4</v>
+      </c>
+      <c r="D18" t="n">
+        <v>3.02</v>
+      </c>
+      <c r="E18" t="n">
+        <v>2.74</v>
+      </c>
+      <c r="H18" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1586,6 +1790,18 @@
           <t>BACH</t>
         </is>
       </c>
+      <c r="C19" t="n">
+        <v>25</v>
+      </c>
+      <c r="D19" t="n">
+        <v>2.52</v>
+      </c>
+      <c r="E19" t="n">
+        <v>6.56</v>
+      </c>
+      <c r="H19" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1598,6 +1814,18 @@
           <t>BACH</t>
         </is>
       </c>
+      <c r="C20" t="n">
+        <v>52.6</v>
+      </c>
+      <c r="D20" t="n">
+        <v>2.17</v>
+      </c>
+      <c r="E20" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="H20" t="n">
+        <v>19</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1610,6 +1838,18 @@
           <t>BACH</t>
         </is>
       </c>
+      <c r="C21" t="n">
+        <v>29.2</v>
+      </c>
+      <c r="D21" t="n">
+        <v>2.49</v>
+      </c>
+      <c r="E21" t="n">
+        <v>4.65</v>
+      </c>
+      <c r="H21" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1622,6 +1862,18 @@
           <t>CFGM</t>
         </is>
       </c>
+      <c r="C22" t="n">
+        <v>40</v>
+      </c>
+      <c r="D22" t="n">
+        <v>3.72</v>
+      </c>
+      <c r="E22" t="n">
+        <v>19.05</v>
+      </c>
+      <c r="H22" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1634,6 +1886,18 @@
           <t>CFGM</t>
         </is>
       </c>
+      <c r="C23" t="n">
+        <v>31.2</v>
+      </c>
+      <c r="D23" t="n">
+        <v>2.01</v>
+      </c>
+      <c r="E23" t="n">
+        <v>15.08</v>
+      </c>
+      <c r="H23" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1646,6 +1910,18 @@
           <t>CFGM</t>
         </is>
       </c>
+      <c r="C24" t="n">
+        <v>57.9</v>
+      </c>
+      <c r="D24" t="n">
+        <v>3.49</v>
+      </c>
+      <c r="E24" t="n">
+        <v>17.23</v>
+      </c>
+      <c r="H24" t="n">
+        <v>19</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1658,6 +1934,18 @@
           <t>CFGM</t>
         </is>
       </c>
+      <c r="C25" t="n">
+        <v>100</v>
+      </c>
+      <c r="D25" t="n">
+        <v>3.49</v>
+      </c>
+      <c r="E25" t="n">
+        <v>14</v>
+      </c>
+      <c r="H25" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1670,6 +1958,18 @@
           <t>CFGM</t>
         </is>
       </c>
+      <c r="C26" t="n">
+        <v>61.5</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="E26" t="n">
+        <v>11.06</v>
+      </c>
+      <c r="H26" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1682,6 +1982,18 @@
           <t>CFGM</t>
         </is>
       </c>
+      <c r="C27" t="n">
+        <v>81.8</v>
+      </c>
+      <c r="D27" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="E27" t="n">
+        <v>8.69</v>
+      </c>
+      <c r="H27" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1694,6 +2006,18 @@
           <t>CFGS</t>
         </is>
       </c>
+      <c r="C28" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="D28" t="n">
+        <v>1.81</v>
+      </c>
+      <c r="E28" t="n">
+        <v>6.42</v>
+      </c>
+      <c r="H28" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1706,6 +2030,18 @@
           <t>CFGS</t>
         </is>
       </c>
+      <c r="C29" t="n">
+        <v>74.09999999999999</v>
+      </c>
+      <c r="D29" t="n">
+        <v>1.97</v>
+      </c>
+      <c r="E29" t="n">
+        <v>11.54</v>
+      </c>
+      <c r="H29" t="n">
+        <v>27</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1718,6 +2054,18 @@
           <t>CFGS</t>
         </is>
       </c>
+      <c r="C30" t="n">
+        <v>67.90000000000001</v>
+      </c>
+      <c r="D30" t="n">
+        <v>4.27</v>
+      </c>
+      <c r="E30" t="n">
+        <v>10.48</v>
+      </c>
+      <c r="H30" t="n">
+        <v>28</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1730,6 +2078,18 @@
           <t>CFGS</t>
         </is>
       </c>
+      <c r="C31" t="n">
+        <v>57.7</v>
+      </c>
+      <c r="D31" t="n">
+        <v>1.48</v>
+      </c>
+      <c r="E31" t="n">
+        <v>11.84</v>
+      </c>
+      <c r="H31" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1742,6 +2102,18 @@
           <t>CFGS</t>
         </is>
       </c>
+      <c r="C32" t="n">
+        <v>28</v>
+      </c>
+      <c r="D32" t="n">
+        <v>3.14</v>
+      </c>
+      <c r="E32" t="n">
+        <v>6.93</v>
+      </c>
+      <c r="H32" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1754,6 +2126,18 @@
           <t>CFGS</t>
         </is>
       </c>
+      <c r="C33" t="n">
+        <v>93.3</v>
+      </c>
+      <c r="D33" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="E33" t="n">
+        <v>4.56</v>
+      </c>
+      <c r="H33" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1766,6 +2150,18 @@
           <t>CFGS</t>
         </is>
       </c>
+      <c r="C34" t="n">
+        <v>100</v>
+      </c>
+      <c r="D34" t="n">
+        <v>1.51</v>
+      </c>
+      <c r="E34" t="n">
+        <v>5.51</v>
+      </c>
+      <c r="H34" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1778,6 +2174,18 @@
           <t>CFGS</t>
         </is>
       </c>
+      <c r="C35" t="n">
+        <v>90.90000000000001</v>
+      </c>
+      <c r="D35" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="E35" t="n">
+        <v>7.58</v>
+      </c>
+      <c r="H35" t="n">
+        <v>22</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1790,6 +2198,18 @@
           <t>CFGS</t>
         </is>
       </c>
+      <c r="C36" t="n">
+        <v>94.7</v>
+      </c>
+      <c r="D36" t="n">
+        <v>1.46</v>
+      </c>
+      <c r="E36" t="n">
+        <v>5.62</v>
+      </c>
+      <c r="H36" t="n">
+        <v>19</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1802,9 +2222,45 @@
           <t>CFGS</t>
         </is>
       </c>
+      <c r="C37" t="n">
+        <v>58.3</v>
+      </c>
+      <c r="D37" t="n">
+        <v>1.68</v>
+      </c>
+      <c r="E37" t="n">
+        <v>16.29</v>
+      </c>
+      <c r="H37" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>3DAM</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>CFGS</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>100</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="H38" t="n">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1816,17 +2272,17 @@
   </sheetPr>
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="0"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="4" min="4" style="2" width="11.33203125"/>
-    <col customWidth="1" max="7" min="7" style="2" width="18.83203125"/>
+    <col width="11.33203125" bestFit="1" customWidth="1" style="2" min="4" max="4"/>
+    <col width="18.83203125" customWidth="1" style="2" min="7" max="7"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1">
+    <row r="1" customFormat="1" s="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>grupo</t>
@@ -1868,7 +2324,7 @@
         </is>
       </c>
     </row>
-    <row r="2" s="2">
+    <row r="2">
       <c r="A2" t="inlineStr">
         <is>
           <t>ESO1A</t>
@@ -1880,7 +2336,7 @@
         </is>
       </c>
     </row>
-    <row r="3" s="2">
+    <row r="3">
       <c r="A3" t="inlineStr">
         <is>
           <t>ESO1B</t>
@@ -1892,7 +2348,7 @@
         </is>
       </c>
     </row>
-    <row r="4" s="2">
+    <row r="4">
       <c r="A4" t="inlineStr">
         <is>
           <t>ESO1C</t>
@@ -1904,7 +2360,7 @@
         </is>
       </c>
     </row>
-    <row r="5" s="2">
+    <row r="5">
       <c r="A5" t="inlineStr">
         <is>
           <t>ESO1D</t>
@@ -1916,7 +2372,7 @@
         </is>
       </c>
     </row>
-    <row r="6" s="2">
+    <row r="6">
       <c r="A6" t="inlineStr">
         <is>
           <t>ESO2A</t>
@@ -1928,7 +2384,7 @@
         </is>
       </c>
     </row>
-    <row r="7" s="2">
+    <row r="7">
       <c r="A7" t="inlineStr">
         <is>
           <t>ESO2B</t>
@@ -1940,7 +2396,7 @@
         </is>
       </c>
     </row>
-    <row r="8" s="2">
+    <row r="8">
       <c r="A8" t="inlineStr">
         <is>
           <t>ESO2C</t>
@@ -1952,7 +2408,7 @@
         </is>
       </c>
     </row>
-    <row r="9" s="2">
+    <row r="9">
       <c r="A9" t="inlineStr">
         <is>
           <t>ESO3A</t>
@@ -1964,7 +2420,7 @@
         </is>
       </c>
     </row>
-    <row r="10" s="2">
+    <row r="10">
       <c r="A10" t="inlineStr">
         <is>
           <t>ESO3B</t>
@@ -1976,7 +2432,7 @@
         </is>
       </c>
     </row>
-    <row r="11" s="2">
+    <row r="11">
       <c r="A11" t="inlineStr">
         <is>
           <t>ESO3C</t>
@@ -1988,7 +2444,7 @@
         </is>
       </c>
     </row>
-    <row r="12" s="2">
+    <row r="12">
       <c r="A12" t="inlineStr">
         <is>
           <t>ESO3D</t>
@@ -2000,7 +2456,7 @@
         </is>
       </c>
     </row>
-    <row r="13" s="2">
+    <row r="13">
       <c r="A13" t="inlineStr">
         <is>
           <t>ESO4A</t>
@@ -2012,7 +2468,7 @@
         </is>
       </c>
     </row>
-    <row r="14" s="2">
+    <row r="14">
       <c r="A14" t="inlineStr">
         <is>
           <t>ESO4B</t>
@@ -2024,7 +2480,7 @@
         </is>
       </c>
     </row>
-    <row r="15" s="2">
+    <row r="15">
       <c r="A15" t="inlineStr">
         <is>
           <t>ESO4C</t>
@@ -2337,6 +2793,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add analysis of C1920-E3
</commit_message>
<xml_diff>
--- a/data/C1920.xlsx
+++ b/data/C1920.xlsx
@@ -2335,6 +2335,18 @@
           <t>ESO</t>
         </is>
       </c>
+      <c r="C2" t="n">
+        <v>57.7</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2.54</v>
+      </c>
+      <c r="H2" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -2347,6 +2359,18 @@
           <t>ESO</t>
         </is>
       </c>
+      <c r="C3" t="n">
+        <v>61.5</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="E3" t="n">
+        <v>3</v>
+      </c>
+      <c r="H3" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -2359,6 +2383,18 @@
           <t>ESO</t>
         </is>
       </c>
+      <c r="C4" t="n">
+        <v>67.90000000000001</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2.12</v>
+      </c>
+      <c r="H4" t="n">
+        <v>28</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -2371,6 +2407,18 @@
           <t>ESO</t>
         </is>
       </c>
+      <c r="C5" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="E5" t="n">
+        <v>3.29</v>
+      </c>
+      <c r="H5" t="n">
+        <v>27</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -2383,6 +2431,18 @@
           <t>ESO</t>
         </is>
       </c>
+      <c r="C6" t="n">
+        <v>88</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="E6" t="n">
+        <v>4.11</v>
+      </c>
+      <c r="H6" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -2395,6 +2455,18 @@
           <t>ESO</t>
         </is>
       </c>
+      <c r="C7" t="n">
+        <v>80</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="E7" t="n">
+        <v>3.11</v>
+      </c>
+      <c r="H7" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -2407,6 +2479,18 @@
           <t>ESO</t>
         </is>
       </c>
+      <c r="C8" t="n">
+        <v>16.7</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="E8" t="n">
+        <v>4.62</v>
+      </c>
+      <c r="H8" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -2419,6 +2503,18 @@
           <t>ESO</t>
         </is>
       </c>
+      <c r="C9" t="n">
+        <v>88.5</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1.28</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1.92</v>
+      </c>
+      <c r="H9" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -2431,6 +2527,18 @@
           <t>ESO</t>
         </is>
       </c>
+      <c r="C10" t="n">
+        <v>65.40000000000001</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1.49</v>
+      </c>
+      <c r="E10" t="n">
+        <v>3.01</v>
+      </c>
+      <c r="H10" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -2443,6 +2551,18 @@
           <t>ESO</t>
         </is>
       </c>
+      <c r="C11" t="n">
+        <v>71.40000000000001</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1.77</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1.74</v>
+      </c>
+      <c r="H11" t="n">
+        <v>28</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -2455,6 +2575,18 @@
           <t>ESO</t>
         </is>
       </c>
+      <c r="C12" t="n">
+        <v>33.3</v>
+      </c>
+      <c r="D12" t="n">
+        <v>2.29</v>
+      </c>
+      <c r="E12" t="n">
+        <v>3.05</v>
+      </c>
+      <c r="H12" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2467,6 +2599,18 @@
           <t>ESO</t>
         </is>
       </c>
+      <c r="C13" t="n">
+        <v>87.5</v>
+      </c>
+      <c r="D13" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="E13" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="H13" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2479,6 +2623,18 @@
           <t>ESO</t>
         </is>
       </c>
+      <c r="C14" t="n">
+        <v>70.40000000000001</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1.87</v>
+      </c>
+      <c r="E14" t="n">
+        <v>2.15</v>
+      </c>
+      <c r="H14" t="n">
+        <v>27</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2491,6 +2647,18 @@
           <t>ESO</t>
         </is>
       </c>
+      <c r="C15" t="n">
+        <v>56</v>
+      </c>
+      <c r="D15" t="n">
+        <v>2.32</v>
+      </c>
+      <c r="E15" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="H15" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2503,6 +2671,18 @@
           <t>FPB</t>
         </is>
       </c>
+      <c r="C16" t="n">
+        <v>73.3</v>
+      </c>
+      <c r="D16" t="n">
+        <v>3.44</v>
+      </c>
+      <c r="E16" t="n">
+        <v>12.8</v>
+      </c>
+      <c r="H16" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2515,6 +2695,18 @@
           <t>FPB</t>
         </is>
       </c>
+      <c r="C17" t="n">
+        <v>100</v>
+      </c>
+      <c r="D17" t="n">
+        <v>5.45</v>
+      </c>
+      <c r="E17" t="n">
+        <v>13.11</v>
+      </c>
+      <c r="H17" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2527,6 +2719,18 @@
           <t>BACH</t>
         </is>
       </c>
+      <c r="C18" t="n">
+        <v>58.8</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E18" t="n">
+        <v>1.72</v>
+      </c>
+      <c r="H18" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2539,6 +2743,18 @@
           <t>BACH</t>
         </is>
       </c>
+      <c r="C19" t="n">
+        <v>50</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1.61</v>
+      </c>
+      <c r="E19" t="n">
+        <v>4.19</v>
+      </c>
+      <c r="H19" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2551,6 +2767,18 @@
           <t>BACH</t>
         </is>
       </c>
+      <c r="C20" t="n">
+        <v>84.2</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="E20" t="n">
+        <v>2.32</v>
+      </c>
+      <c r="H20" t="n">
+        <v>19</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2563,6 +2791,18 @@
           <t>BACH</t>
         </is>
       </c>
+      <c r="C21" t="n">
+        <v>100</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="E21" t="n">
+        <v>2.92</v>
+      </c>
+      <c r="H21" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2575,6 +2815,18 @@
           <t>CFGM</t>
         </is>
       </c>
+      <c r="C22" t="n">
+        <v>40</v>
+      </c>
+      <c r="D22" t="n">
+        <v>2.48</v>
+      </c>
+      <c r="E22" t="n">
+        <v>12.72</v>
+      </c>
+      <c r="H22" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2587,6 +2839,18 @@
           <t>CFGM</t>
         </is>
       </c>
+      <c r="C23" t="n">
+        <v>56.2</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="E23" t="n">
+        <v>9.74</v>
+      </c>
+      <c r="H23" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2599,6 +2863,18 @@
           <t>CFGM</t>
         </is>
       </c>
+      <c r="C24" t="n">
+        <v>57.9</v>
+      </c>
+      <c r="D24" t="n">
+        <v>2.24</v>
+      </c>
+      <c r="E24" t="n">
+        <v>11.05</v>
+      </c>
+      <c r="H24" t="n">
+        <v>19</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2611,6 +2887,18 @@
           <t>CFGM</t>
         </is>
       </c>
+      <c r="C25" t="n">
+        <v>100</v>
+      </c>
+      <c r="D25" t="n">
+        <v>2.79</v>
+      </c>
+      <c r="E25" t="n">
+        <v>11.21</v>
+      </c>
+      <c r="H25" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2623,6 +2911,18 @@
           <t>CFGM</t>
         </is>
       </c>
+      <c r="C26" t="n">
+        <v>100</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1.38</v>
+      </c>
+      <c r="E26" t="n">
+        <v>8.970000000000001</v>
+      </c>
+      <c r="H26" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2635,6 +2935,18 @@
           <t>CFGM</t>
         </is>
       </c>
+      <c r="C27" t="n">
+        <v>100</v>
+      </c>
+      <c r="D27" t="n">
+        <v>1.23</v>
+      </c>
+      <c r="E27" t="n">
+        <v>6.73</v>
+      </c>
+      <c r="H27" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2647,6 +2959,18 @@
           <t>CFGS</t>
         </is>
       </c>
+      <c r="C28" t="n">
+        <v>90.90000000000001</v>
+      </c>
+      <c r="D28" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="E28" t="n">
+        <v>4.59</v>
+      </c>
+      <c r="H28" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2659,6 +2983,18 @@
           <t>CFGS</t>
         </is>
       </c>
+      <c r="C29" t="n">
+        <v>81.5</v>
+      </c>
+      <c r="D29" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="E29" t="n">
+        <v>7.35</v>
+      </c>
+      <c r="H29" t="n">
+        <v>27</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2671,6 +3007,18 @@
           <t>CFGS</t>
         </is>
       </c>
+      <c r="C30" t="n">
+        <v>89.3</v>
+      </c>
+      <c r="D30" t="n">
+        <v>2.68</v>
+      </c>
+      <c r="E30" t="n">
+        <v>6.59</v>
+      </c>
+      <c r="H30" t="n">
+        <v>28</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2683,6 +3031,18 @@
           <t>CFGS</t>
         </is>
       </c>
+      <c r="C31" t="n">
+        <v>84</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="E31" t="n">
+        <v>7.89</v>
+      </c>
+      <c r="H31" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -2695,6 +3055,18 @@
           <t>CFGS</t>
         </is>
       </c>
+      <c r="C32" t="n">
+        <v>92</v>
+      </c>
+      <c r="D32" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="E32" t="n">
+        <v>4.53</v>
+      </c>
+      <c r="H32" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2707,6 +3079,18 @@
           <t>CFGS</t>
         </is>
       </c>
+      <c r="C33" t="n">
+        <v>100</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="E33" t="n">
+        <v>3.67</v>
+      </c>
+      <c r="H33" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -2719,6 +3103,18 @@
           <t>CFGS</t>
         </is>
       </c>
+      <c r="C34" t="n">
+        <v>100</v>
+      </c>
+      <c r="D34" t="n">
+        <v>1.19</v>
+      </c>
+      <c r="E34" t="n">
+        <v>4.33</v>
+      </c>
+      <c r="H34" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2731,6 +3127,18 @@
           <t>CFGS</t>
         </is>
       </c>
+      <c r="C35" t="n">
+        <v>100</v>
+      </c>
+      <c r="D35" t="n">
+        <v>1.46</v>
+      </c>
+      <c r="E35" t="n">
+        <v>5.68</v>
+      </c>
+      <c r="H35" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2743,6 +3151,18 @@
           <t>CFGS</t>
         </is>
       </c>
+      <c r="C36" t="n">
+        <v>100</v>
+      </c>
+      <c r="D36" t="n">
+        <v>1.27</v>
+      </c>
+      <c r="E36" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="H36" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -2755,6 +3175,18 @@
           <t>CFGS</t>
         </is>
       </c>
+      <c r="C37" t="n">
+        <v>100</v>
+      </c>
+      <c r="D37" t="n">
+        <v>1.43</v>
+      </c>
+      <c r="E37" t="n">
+        <v>13.82</v>
+      </c>
+      <c r="H37" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2767,6 +3199,18 @@
           <t>CFGS</t>
         </is>
       </c>
+      <c r="C38" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="H38" t="n">
+        <v>38</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2779,6 +3223,18 @@
           <t>CFGS</t>
         </is>
       </c>
+      <c r="C39" t="n">
+        <v>71.40000000000001</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="H39" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2790,6 +3246,18 @@
         <is>
           <t>CFGS</t>
         </is>
+      </c>
+      <c r="C40" t="n">
+        <v>100</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="H40" t="n">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>